<commit_message>
update on MF feasability
</commit_message>
<xml_diff>
--- a/src/databases/logisticsDB_vessel_python.xlsx
+++ b/src/databases/logisticsDB_vessel_python.xlsx
@@ -1636,15 +1636,17 @@
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+      <selection activeCell="C5" activeCellId="1" pane="topLeft" sqref="M3 C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9607843137255"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -1916,76 +1918,76 @@
   <dimension ref="A2:CQ59"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A52" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="L38" activeCellId="0" pane="topLeft" sqref="L38"/>
+      <selection activeCell="L38" activeCellId="1" pane="topLeft" sqref="M3 L38"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.9058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="24.1450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="20.8313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="15.043137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="9" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="23.7137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="21.1098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="7.8156862745098"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="6.94117647058824"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="7.95294117647059"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="9.10588235294118"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="5.63529411764706"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="7.51372549019608"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="7.37254901960784"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="8" width="8.53333333333333"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="10.4117647058824"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="7.8156862745098"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="8" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="9.10588235294118"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="8.37647058823529"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="8" width="7.37254901960784"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="8" width="8.37647058823529"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="8" width="8.97254901960784"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="8" width="7.37254901960784"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="8" width="7.51372549019608"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="8" width="8.24705882352941"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="8" width="8.53333333333333"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="8" width="8.24705882352941"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="8" width="9.98039215686275"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="8" width="8.37647058823529"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="8" width="8.97254901960784"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="8" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="8" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="8" width="16.0470588235294"/>
-    <col collapsed="false" hidden="false" max="54" min="51" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="8" width="11.278431372549"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="8" width="10.9843137254902"/>
-    <col collapsed="false" hidden="false" max="58" min="57" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="8" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="8" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="8" width="9.54509803921569"/>
-    <col collapsed="false" hidden="false" max="69" min="63" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="8" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="8" width="7.8156862745098"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="8" width="8.24705882352941"/>
-    <col collapsed="false" hidden="false" max="81" min="74" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="8" width="15.043137254902"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="8" width="13.8745098039216"/>
-    <col collapsed="false" hidden="false" max="94" min="84" style="8" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="8" width="50.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="96" style="8" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.9686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="24.243137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="20.9176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="15.1098039215686"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="9" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="23.8156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.556862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="21.1960784313725"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.556862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="7.84313725490196"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="6.96862745098039"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="7.98039215686275"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="9.14117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="5.65882352941177"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="7.54509803921569"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="7.4"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="8" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="10.4549019607843"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="7.84313725490196"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="8" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="9.14117647058824"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="8" width="7.4"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="8" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="8" width="9.0078431372549"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="8" width="7.4"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="8" width="7.54509803921569"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="8" width="8.28235294117647"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="8" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="8" width="8.28235294117647"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="8" width="10.0196078431373"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="8" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="8" width="9.0078431372549"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="8" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="8" width="12.1960784313725"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="8" width="16.1137254901961"/>
+    <col collapsed="false" hidden="false" max="54" min="51" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="8" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="8" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="58" min="57" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="8" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="8" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="8" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="69" min="63" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="8" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="8" width="7.84313725490196"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="8" width="8.28235294117647"/>
+    <col collapsed="false" hidden="false" max="81" min="74" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="8" width="15.1098039215686"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="8" width="13.9333333333333"/>
+    <col collapsed="false" hidden="false" max="94" min="84" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="8" width="50.3960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="96" style="8" width="9.30196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="2">
@@ -10793,66 +10795,66 @@
   </sheetPr>
   <dimension ref="A1:CH52"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="M3" activeCellId="0" pane="topLeft" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6274509803922"/>
-    <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6274509803922"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5176470588235"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.4745098039216"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="19" min="16" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.9843137254902"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.5960784313726"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.1647058823529"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.9843137254902"/>
-    <col collapsed="false" hidden="false" max="28" min="26" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9843137254902"/>
-    <col collapsed="false" hidden="false" max="32" min="30" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.9843137254902"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.556862745098"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.1372549019608"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.4745098039216"/>
-    <col collapsed="false" hidden="false" max="47" min="46" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="13.0078431372549"/>
-    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="11.1372549019608"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="13.0078431372549"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="12.5843137254902"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="13.5960784313726"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="15.043137254902"/>
-    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="14.3137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6941176470588"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5960784313726"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5411764705882"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0078431372549"/>
+    <col collapsed="false" hidden="false" max="19" min="16" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.2235294117647"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="32" min="30" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.1882352941176"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.3647058823529"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.9098039215686"/>
+    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.5411764705882"/>
+    <col collapsed="false" hidden="false" max="47" min="46" style="0" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.3411764705882"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="13.7960784313726"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="13.0666666666667"/>
+    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="13.3647058823529"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="11.1882352941176"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="14.8078431372549"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="11.9098039215686"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="10.3098039215686"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="12.1960784313725"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="13.0666666666667"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="12.6352941176471"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="12.3411764705882"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.7960784313726"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="15.1098039215686"/>
+    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="14.956862745098"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="13.3647058823529"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="14.3686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="86.25" outlineLevel="0" r="1">
@@ -11200,7 +11202,7 @@
       <c r="CD2" s="86"/>
       <c r="CE2" s="86"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3" s="87">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="3" s="87">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
@@ -11229,7 +11231,7 @@
       <c r="J3" s="66"/>
       <c r="K3" s="66"/>
       <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="M3" s="0"/>
       <c r="N3" s="66" t="n">
         <v>2320</v>
       </c>
@@ -12639,7 +12641,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
       <c r="A14" s="3" t="n">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Fr*aking Matching almost but not yet completly finished... but believe i will be able to finish tomorrow...
</commit_message>
<xml_diff>
--- a/src/databases/logisticsDB_vessel_python.xlsx
+++ b/src/databases/logisticsDB_vessel_python.xlsx
@@ -948,7 +948,7 @@
     <numFmt formatCode="@" numFmtId="165"/>
     <numFmt formatCode="0" numFmtId="166"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -1109,6 +1109,12 @@
       <charset val="1"/>
       <family val="2"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1292,7 +1298,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -1547,6 +1553,9 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
@@ -1636,17 +1645,17 @@
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="1" pane="topLeft" sqref="M3 C5"/>
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.756862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.278431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -1918,76 +1927,76 @@
   <dimension ref="A2:CQ59"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A52" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="L38" activeCellId="1" pane="topLeft" sqref="M3 L38"/>
+      <selection activeCell="L38" activeCellId="0" pane="topLeft" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.9686274509804"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="24.243137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="20.9176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="15.1098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="9" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="23.8156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.556862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="21.1960784313725"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.556862745098"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="7.84313725490196"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="6.96862745098039"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="7.98039215686275"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="9.14117647058824"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="5.65882352941177"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="7.54509803921569"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="7.4"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="11.7686274509804"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="8" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="10.4549019607843"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="7.84313725490196"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="8" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="9.14117647058824"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="8.41176470588235"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="8" width="7.4"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="8" width="8.41176470588235"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="8" width="9.0078431372549"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="8" width="7.4"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="8" width="7.54509803921569"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="8" width="8.28235294117647"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="8" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="8" width="8.28235294117647"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="8" width="10.0196078431373"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="8" width="8.41176470588235"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="8" width="9.0078431372549"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="8" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="8" width="12.1960784313725"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="8" width="16.1137254901961"/>
-    <col collapsed="false" hidden="false" max="54" min="51" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="8" width="11.321568627451"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="8" width="11.0274509803922"/>
-    <col collapsed="false" hidden="false" max="58" min="57" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="8" width="12.921568627451"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="8" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="8" width="9.58823529411765"/>
-    <col collapsed="false" hidden="false" max="69" min="63" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="8" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="8" width="7.84313725490196"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="8" width="8.28235294117647"/>
-    <col collapsed="false" hidden="false" max="81" min="74" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="8" width="15.1098039215686"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="8" width="13.9333333333333"/>
-    <col collapsed="false" hidden="false" max="94" min="84" style="8" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="8" width="50.3960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="96" style="8" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="16.0352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="24.3450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="21.0039215686275"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="15.1725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="9" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="23.9137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.6274509803922"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="21.2823529411765"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.6274509803922"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="7.87450980392157"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="7"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="8.01176470588235"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="5.68627450980392"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="7.42745098039216"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="11.8156862745098"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="8" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="10.4980392156863"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="7.87450980392157"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="8" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="8.44705882352941"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="8" width="7.42745098039216"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="8" width="8.44705882352941"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="8" width="9.04313725490196"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="8" width="7.42745098039216"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="8" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="8" width="8.31764705882353"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="8" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="8" width="8.31764705882353"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="8" width="10.0588235294118"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="8" width="8.44705882352941"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="8" width="9.04313725490196"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="8" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="8" width="12.2470588235294"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="8" width="16.1764705882353"/>
+    <col collapsed="false" hidden="false" max="54" min="51" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="8" width="11.3647058823529"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="8" width="11.0705882352941"/>
+    <col collapsed="false" hidden="false" max="58" min="57" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="8" width="12.9803921568627"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="8" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="8" width="9.62352941176471"/>
+    <col collapsed="false" hidden="false" max="69" min="63" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="8" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="8" width="7.87450980392157"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="8" width="8.31764705882353"/>
+    <col collapsed="false" hidden="false" max="81" min="74" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="8" width="15.1725490196078"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="8" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="94" min="84" style="8" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="8" width="50.6039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="96" style="8" width="9.34509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="2">
@@ -10795,66 +10804,66 @@
   </sheetPr>
   <dimension ref="A1:CH52"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="M3" activeCellId="0" pane="topLeft" sqref="M3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="AR1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="BA1" activeCellId="0" pane="topLeft" sqref="BA1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5960784313726"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5411764705882"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0078431372549"/>
-    <col collapsed="false" hidden="false" max="19" min="16" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0274509803922"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.2235294117647"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.0274509803922"/>
-    <col collapsed="false" hidden="false" max="28" min="26" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.0274509803922"/>
-    <col collapsed="false" hidden="false" max="32" min="30" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="11.0274509803922"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.3647058823529"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.7686274509804"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.9098039215686"/>
-    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="14.2274509803922"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.5411764705882"/>
-    <col collapsed="false" hidden="false" max="47" min="46" style="0" width="14.2274509803922"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.3411764705882"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="13.7960784313726"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="13.0666666666667"/>
-    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="12.921568627451"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="13.3647058823529"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="14.8078431372549"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="11.9098039215686"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="10.3098039215686"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.7686274509804"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="12.1960784313725"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="13.0666666666667"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="11.7686274509804"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="12.6352941176471"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="10.7411764705882"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="12.3411764705882"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.7960784313726"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="15.1098039215686"/>
-    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="14.956862745098"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="13.3647058823529"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="14.3686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.756862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.756862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.678431372549"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0862745098039"/>
+    <col collapsed="false" hidden="false" max="19" min="16" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0705882352941"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.7098039215686"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.2823529411765"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.0705882352941"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.0705882352941"/>
+    <col collapsed="false" hidden="false" max="32" min="30" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="11.0705882352941"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.6470588235294"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.8156862745098"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="14.2862745098039"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.6039215686275"/>
+    <col collapsed="false" hidden="false" max="47" min="46" style="0" width="14.2862745098039"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="13.8549019607843"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="12.9803921568627"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="10.3529411764706"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.8156862745098"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="12.2470588235294"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="11.8156862745098"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="12.6862745098039"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="10.7843137254902"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="13.7098039215686"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.8549019607843"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="15.1725490196078"/>
+    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="15.0156862745098"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="86.25" outlineLevel="0" r="1">
@@ -11006,7 +11015,7 @@
       <c r="AX1" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="AY1" s="84" t="s">
+      <c r="AY1" s="85" t="s">
         <v>258</v>
       </c>
       <c r="AZ1" s="84" t="s">
@@ -11081,19 +11090,19 @@
       <c r="BW1" s="84" t="s">
         <v>282</v>
       </c>
-      <c r="BX1" s="85"/>
-      <c r="BY1" s="85"/>
-      <c r="BZ1" s="85"/>
-      <c r="CA1" s="85"/>
-      <c r="CB1" s="85"/>
-      <c r="CC1" s="85"/>
-      <c r="CD1" s="85"/>
-      <c r="CE1" s="85"/>
-      <c r="CF1" s="85"/>
-      <c r="CG1" s="85"/>
-      <c r="CH1" s="85"/>
+      <c r="BX1" s="86"/>
+      <c r="BY1" s="86"/>
+      <c r="BZ1" s="86"/>
+      <c r="CA1" s="86"/>
+      <c r="CB1" s="86"/>
+      <c r="CC1" s="86"/>
+      <c r="CD1" s="86"/>
+      <c r="CE1" s="86"/>
+      <c r="CF1" s="86"/>
+      <c r="CG1" s="86"/>
+      <c r="CH1" s="86"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2" s="87">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2" s="88">
       <c r="A2" s="61" t="n">
         <v>1</v>
       </c>
@@ -11193,16 +11202,16 @@
       <c r="BW2" s="64" t="n">
         <v>400</v>
       </c>
-      <c r="BX2" s="86"/>
-      <c r="BY2" s="86"/>
-      <c r="BZ2" s="86"/>
-      <c r="CA2" s="86"/>
-      <c r="CB2" s="86"/>
-      <c r="CC2" s="86"/>
-      <c r="CD2" s="86"/>
-      <c r="CE2" s="86"/>
+      <c r="BX2" s="87"/>
+      <c r="BY2" s="87"/>
+      <c r="BZ2" s="87"/>
+      <c r="CA2" s="87"/>
+      <c r="CB2" s="87"/>
+      <c r="CC2" s="87"/>
+      <c r="CD2" s="87"/>
+      <c r="CE2" s="87"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="3" s="87">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3" s="88">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
@@ -11231,7 +11240,6 @@
       <c r="J3" s="66"/>
       <c r="K3" s="66"/>
       <c r="L3" s="66"/>
-      <c r="M3" s="0"/>
       <c r="N3" s="66" t="n">
         <v>2320</v>
       </c>
@@ -11303,7 +11311,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4" s="87">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4" s="88">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
select_ve working / needs to be checked again
</commit_message>
<xml_diff>
--- a/src/databases/logisticsDB_vessel_python.xlsx
+++ b/src/databases/logisticsDB_vessel_python.xlsx
@@ -1502,65 +1502,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1588,6 +1540,54 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,6 +1790,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2106,12 +2154,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="4" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2120,19 +2168,19 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="70"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="70" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -2143,8 +2191,8 @@
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="67"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
@@ -2153,8 +2201,8 @@
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="67" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="70" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -2165,8 +2213,8 @@
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="67"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2175,20 +2223,20 @@
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="69"/>
+      <c r="D9" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="67"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="D10" s="70" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2199,8 +2247,8 @@
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="67"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2209,70 +2257,70 @@
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="67" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="67"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="67" t="s">
+      <c r="C13" s="69"/>
+      <c r="D13" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="67"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="67" t="s">
+      <c r="C14" s="69"/>
+      <c r="D14" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="67"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="67" t="s">
+      <c r="C15" s="69"/>
+      <c r="D15" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="67"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>14</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="67" t="s">
+      <c r="C17" s="69"/>
+      <c r="D17" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="67"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>15</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="67" t="s">
+      <c r="C18" s="69"/>
+      <c r="D18" s="70" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2283,8 +2331,8 @@
       <c r="B19" s="3">
         <v>16</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="67"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="5" t="s">
         <v>25</v>
       </c>
@@ -2293,21 +2341,21 @@
       <c r="B20" s="6">
         <v>17</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="67" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>18</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="67" t="s">
+      <c r="C21" s="69"/>
+      <c r="D21" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="67"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
@@ -2316,10 +2364,10 @@
       <c r="C22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
@@ -2328,25 +2376,13 @@
       <c r="C23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="67" t="s">
+      <c r="D23" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="67"/>
+      <c r="E23" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="C16:C21"/>
@@ -2355,6 +2391,18 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2440,382 +2488,382 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:95" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="87"/>
-      <c r="AJ2" s="87"/>
-      <c r="AK2" s="87"/>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="87"/>
-      <c r="AN2" s="87"/>
-      <c r="AO2" s="87"/>
-      <c r="AP2" s="87"/>
-      <c r="AQ2" s="87"/>
-      <c r="AR2" s="87"/>
-      <c r="AS2" s="87"/>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="87"/>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="87"/>
-      <c r="AX2" s="87"/>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="87"/>
-      <c r="BB2" s="87"/>
-      <c r="BC2" s="87"/>
-      <c r="BD2" s="87"/>
-      <c r="BE2" s="87"/>
-      <c r="BF2" s="87"/>
-      <c r="BG2" s="87"/>
-      <c r="BH2" s="87"/>
-      <c r="BI2" s="87"/>
-      <c r="BJ2" s="87"/>
-      <c r="BK2" s="87"/>
-      <c r="BL2" s="87"/>
-      <c r="BM2" s="87"/>
-      <c r="BN2" s="87"/>
-      <c r="BO2" s="87"/>
-      <c r="BP2" s="87"/>
-      <c r="BQ2" s="87"/>
-      <c r="BR2" s="87"/>
-      <c r="BS2" s="87"/>
-      <c r="BT2" s="87"/>
-      <c r="BU2" s="87"/>
-      <c r="BV2" s="87"/>
-      <c r="BW2" s="87"/>
-      <c r="BX2" s="87"/>
-      <c r="BY2" s="87"/>
-      <c r="BZ2" s="87"/>
-      <c r="CA2" s="87"/>
-      <c r="CB2" s="87"/>
-      <c r="CC2" s="87"/>
-      <c r="CD2" s="87"/>
-      <c r="CE2" s="87"/>
-      <c r="CF2" s="88"/>
-      <c r="CG2" s="88"/>
-      <c r="CH2" s="88"/>
-      <c r="CI2" s="88"/>
-      <c r="CJ2" s="88"/>
-      <c r="CK2" s="88"/>
-      <c r="CL2" s="88"/>
-      <c r="CM2" s="88"/>
-      <c r="CN2" s="88"/>
-      <c r="CO2" s="88"/>
-      <c r="CP2" s="88"/>
-      <c r="CQ2" s="88"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="71"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+      <c r="AT2" s="71"/>
+      <c r="AU2" s="71"/>
+      <c r="AV2" s="71"/>
+      <c r="AW2" s="71"/>
+      <c r="AX2" s="71"/>
+      <c r="AY2" s="71"/>
+      <c r="AZ2" s="71"/>
+      <c r="BA2" s="71"/>
+      <c r="BB2" s="71"/>
+      <c r="BC2" s="71"/>
+      <c r="BD2" s="71"/>
+      <c r="BE2" s="71"/>
+      <c r="BF2" s="71"/>
+      <c r="BG2" s="71"/>
+      <c r="BH2" s="71"/>
+      <c r="BI2" s="71"/>
+      <c r="BJ2" s="71"/>
+      <c r="BK2" s="71"/>
+      <c r="BL2" s="71"/>
+      <c r="BM2" s="71"/>
+      <c r="BN2" s="71"/>
+      <c r="BO2" s="71"/>
+      <c r="BP2" s="71"/>
+      <c r="BQ2" s="71"/>
+      <c r="BR2" s="71"/>
+      <c r="BS2" s="71"/>
+      <c r="BT2" s="71"/>
+      <c r="BU2" s="71"/>
+      <c r="BV2" s="71"/>
+      <c r="BW2" s="71"/>
+      <c r="BX2" s="71"/>
+      <c r="BY2" s="71"/>
+      <c r="BZ2" s="71"/>
+      <c r="CA2" s="71"/>
+      <c r="CB2" s="71"/>
+      <c r="CC2" s="71"/>
+      <c r="CD2" s="71"/>
+      <c r="CE2" s="71"/>
+      <c r="CF2" s="72"/>
+      <c r="CG2" s="72"/>
+      <c r="CH2" s="72"/>
+      <c r="CI2" s="72"/>
+      <c r="CJ2" s="72"/>
+      <c r="CK2" s="72"/>
+      <c r="CL2" s="72"/>
+      <c r="CM2" s="72"/>
+      <c r="CN2" s="72"/>
+      <c r="CO2" s="72"/>
+      <c r="CP2" s="72"/>
+      <c r="CQ2" s="72"/>
     </row>
     <row r="3" spans="1:95" s="9" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="90" t="s">
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="90"/>
-      <c r="L3" s="91" t="s">
+      <c r="K3" s="74"/>
+      <c r="L3" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="91"/>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="92" t="s">
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+      <c r="U3" s="75"/>
+      <c r="V3" s="75"/>
+      <c r="W3" s="75"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="75"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="92"/>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="92"/>
-      <c r="AI3" s="92"/>
-      <c r="AJ3" s="92"/>
-      <c r="AK3" s="92"/>
-      <c r="AL3" s="92"/>
-      <c r="AM3" s="92"/>
-      <c r="AN3" s="92"/>
-      <c r="AO3" s="92"/>
-      <c r="AP3" s="93" t="s">
+      <c r="AE3" s="76"/>
+      <c r="AF3" s="76"/>
+      <c r="AG3" s="76"/>
+      <c r="AH3" s="76"/>
+      <c r="AI3" s="76"/>
+      <c r="AJ3" s="76"/>
+      <c r="AK3" s="76"/>
+      <c r="AL3" s="76"/>
+      <c r="AM3" s="76"/>
+      <c r="AN3" s="76"/>
+      <c r="AO3" s="76"/>
+      <c r="AP3" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="AQ3" s="93"/>
-      <c r="AR3" s="93"/>
-      <c r="AS3" s="93"/>
-      <c r="AT3" s="93"/>
-      <c r="AU3" s="93"/>
-      <c r="AV3" s="93"/>
-      <c r="AW3" s="93"/>
-      <c r="AX3" s="93"/>
-      <c r="AY3" s="93"/>
-      <c r="AZ3" s="93"/>
-      <c r="BA3" s="93"/>
-      <c r="BB3" s="93"/>
-      <c r="BC3" s="93"/>
-      <c r="BD3" s="93"/>
-      <c r="BE3" s="93"/>
-      <c r="BF3" s="93"/>
-      <c r="BG3" s="93"/>
-      <c r="BH3" s="93"/>
-      <c r="BI3" s="93"/>
-      <c r="BJ3" s="93"/>
-      <c r="BK3" s="93"/>
-      <c r="BL3" s="93"/>
-      <c r="BM3" s="93"/>
-      <c r="BN3" s="93"/>
-      <c r="BO3" s="93"/>
-      <c r="BP3" s="93"/>
-      <c r="BQ3" s="93"/>
-      <c r="BR3" s="93"/>
-      <c r="BS3" s="93"/>
-      <c r="BT3" s="93"/>
-      <c r="BU3" s="93"/>
-      <c r="BV3" s="93"/>
-      <c r="BW3" s="93"/>
-      <c r="BX3" s="93"/>
-      <c r="BY3" s="93"/>
-      <c r="BZ3" s="93"/>
-      <c r="CA3" s="93"/>
-      <c r="CB3" s="94" t="s">
+      <c r="AQ3" s="77"/>
+      <c r="AR3" s="77"/>
+      <c r="AS3" s="77"/>
+      <c r="AT3" s="77"/>
+      <c r="AU3" s="77"/>
+      <c r="AV3" s="77"/>
+      <c r="AW3" s="77"/>
+      <c r="AX3" s="77"/>
+      <c r="AY3" s="77"/>
+      <c r="AZ3" s="77"/>
+      <c r="BA3" s="77"/>
+      <c r="BB3" s="77"/>
+      <c r="BC3" s="77"/>
+      <c r="BD3" s="77"/>
+      <c r="BE3" s="77"/>
+      <c r="BF3" s="77"/>
+      <c r="BG3" s="77"/>
+      <c r="BH3" s="77"/>
+      <c r="BI3" s="77"/>
+      <c r="BJ3" s="77"/>
+      <c r="BK3" s="77"/>
+      <c r="BL3" s="77"/>
+      <c r="BM3" s="77"/>
+      <c r="BN3" s="77"/>
+      <c r="BO3" s="77"/>
+      <c r="BP3" s="77"/>
+      <c r="BQ3" s="77"/>
+      <c r="BR3" s="77"/>
+      <c r="BS3" s="77"/>
+      <c r="BT3" s="77"/>
+      <c r="BU3" s="77"/>
+      <c r="BV3" s="77"/>
+      <c r="BW3" s="77"/>
+      <c r="BX3" s="77"/>
+      <c r="BY3" s="77"/>
+      <c r="BZ3" s="77"/>
+      <c r="CA3" s="77"/>
+      <c r="CB3" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="CC3" s="94"/>
-      <c r="CD3" s="94"/>
-      <c r="CE3" s="94"/>
-      <c r="CF3" s="95" t="s">
+      <c r="CC3" s="78"/>
+      <c r="CD3" s="78"/>
+      <c r="CE3" s="78"/>
+      <c r="CF3" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="CG3" s="95"/>
-      <c r="CH3" s="95"/>
-      <c r="CI3" s="95"/>
-      <c r="CJ3" s="95" t="s">
+      <c r="CG3" s="79"/>
+      <c r="CH3" s="79"/>
+      <c r="CI3" s="79"/>
+      <c r="CJ3" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="CK3" s="95"/>
-      <c r="CL3" s="95"/>
-      <c r="CM3" s="95"/>
-      <c r="CN3" s="95" t="s">
+      <c r="CK3" s="79"/>
+      <c r="CL3" s="79"/>
+      <c r="CM3" s="79"/>
+      <c r="CN3" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="CO3" s="95"/>
-      <c r="CP3" s="95"/>
+      <c r="CO3" s="79"/>
+      <c r="CP3" s="79"/>
       <c r="CQ3" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:95" s="9" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="72" t="s">
+      <c r="H4" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="I4" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="84" t="s">
+      <c r="J4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="80" t="s">
+      <c r="L4" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81" t="s">
+      <c r="N4" s="85"/>
+      <c r="O4" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="82" t="s">
+      <c r="P4" s="85"/>
+      <c r="Q4" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="83" t="s">
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="83"/>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="77" t="s">
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="Z4" s="77"/>
+      <c r="Z4" s="88"/>
       <c r="AA4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AB4" s="78" t="s">
+      <c r="AB4" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="79" t="s">
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79" t="s">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79" t="s">
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="90"/>
+      <c r="AL4" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="73" t="s">
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="AQ4" s="73"/>
-      <c r="AR4" s="75" t="s">
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
       <c r="AW4" s="15" t="s">
         <v>62</v>
       </c>
       <c r="AX4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="AY4" s="76" t="s">
+      <c r="AY4" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="AZ4" s="76"/>
-      <c r="BA4" s="76"/>
-      <c r="BB4" s="76"/>
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
       <c r="BC4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="BD4" s="73" t="s">
+      <c r="BD4" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73" t="s">
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="91"/>
+      <c r="BG4" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="73" t="s">
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="BL4" s="73"/>
-      <c r="BM4" s="73"/>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="74" t="s">
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="91"/>
+      <c r="BN4" s="91"/>
+      <c r="BO4" s="91"/>
+      <c r="BP4" s="91"/>
+      <c r="BQ4" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="BR4" s="74"/>
-      <c r="BS4" s="74"/>
-      <c r="BT4" s="74"/>
-      <c r="BU4" s="74"/>
-      <c r="BV4" s="73" t="s">
+      <c r="BR4" s="94"/>
+      <c r="BS4" s="94"/>
+      <c r="BT4" s="94"/>
+      <c r="BU4" s="94"/>
+      <c r="BV4" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="BW4" s="73"/>
-      <c r="BX4" s="73"/>
-      <c r="BY4" s="73"/>
-      <c r="BZ4" s="73" t="s">
+      <c r="BW4" s="91"/>
+      <c r="BX4" s="91"/>
+      <c r="BY4" s="91"/>
+      <c r="BZ4" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="CA4" s="73"/>
-      <c r="CB4" s="71" t="s">
+      <c r="CA4" s="91"/>
+      <c r="CB4" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="CC4" s="71"/>
-      <c r="CD4" s="71" t="s">
+      <c r="CC4" s="95"/>
+      <c r="CD4" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="CE4" s="71"/>
-      <c r="CF4" s="72" t="s">
+      <c r="CE4" s="95"/>
+      <c r="CF4" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="CG4" s="72" t="s">
+      <c r="CG4" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="CH4" s="72" t="s">
+      <c r="CH4" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="CI4" s="72" t="s">
+      <c r="CI4" s="81" t="s">
         <v>77</v>
       </c>
       <c r="CJ4" s="18"/>
@@ -2828,17 +2876,17 @@
       <c r="CQ4" s="22"/>
     </row>
     <row r="5" spans="1:95" s="9" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="85"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="84"/>
       <c r="M5" s="23" t="s">
         <v>78</v>
       </c>
@@ -3052,10 +3100,10 @@
       <c r="CE5" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="CF5" s="72"/>
-      <c r="CG5" s="72"/>
-      <c r="CH5" s="72"/>
-      <c r="CI5" s="72"/>
+      <c r="CF5" s="81"/>
+      <c r="CG5" s="81"/>
+      <c r="CH5" s="81"/>
+      <c r="CI5" s="81"/>
       <c r="CJ5" s="12" t="s">
         <v>138</v>
       </c>
@@ -11179,6 +11227,41 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="CD4:CE4"/>
+    <mergeCell ref="CF4:CF5"/>
+    <mergeCell ref="CG4:CG5"/>
+    <mergeCell ref="CH4:CH5"/>
+    <mergeCell ref="CI4:CI5"/>
+    <mergeCell ref="BK4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BV4:BY4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="CB4:CC4"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AR4:AV4"/>
+    <mergeCell ref="AY4:BB4"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BJ4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:CE2"/>
     <mergeCell ref="CF2:CQ2"/>
     <mergeCell ref="C3:I3"/>
@@ -11190,41 +11273,6 @@
     <mergeCell ref="CF3:CI3"/>
     <mergeCell ref="CJ3:CM3"/>
     <mergeCell ref="CN3:CP3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AH4:AK4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AR4:AV4"/>
-    <mergeCell ref="AY4:BB4"/>
-    <mergeCell ref="BD4:BF4"/>
-    <mergeCell ref="BG4:BJ4"/>
-    <mergeCell ref="BK4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BV4:BY4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="CB4:CC4"/>
-    <mergeCell ref="CD4:CE4"/>
-    <mergeCell ref="CF4:CF5"/>
-    <mergeCell ref="CG4:CG5"/>
-    <mergeCell ref="CH4:CH5"/>
-    <mergeCell ref="CI4:CI5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -11237,8 +11285,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AS5" sqref="AS5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="AP5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AQ21" sqref="AQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13298,7 +13349,9 @@
         <v>0</v>
       </c>
       <c r="AO15" s="40"/>
-      <c r="AP15" s="40"/>
+      <c r="AP15" s="40">
+        <v>0</v>
+      </c>
       <c r="AQ15" s="40"/>
       <c r="AR15" s="40"/>
       <c r="AS15" s="40"/>
@@ -13411,7 +13464,9 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
       <c r="AO16" s="6"/>
-      <c r="AP16" s="6"/>
+      <c r="AP16" s="6">
+        <v>2</v>
+      </c>
       <c r="AQ16" s="6"/>
       <c r="AR16" s="6"/>
       <c r="AS16" s="6"/>
@@ -13534,7 +13589,9 @@
         <v>0</v>
       </c>
       <c r="AO17" s="6"/>
-      <c r="AP17" s="6"/>
+      <c r="AP17" s="6">
+        <v>3</v>
+      </c>
       <c r="AQ17" s="6"/>
       <c r="AR17" s="6"/>
       <c r="AS17" s="6"/>
@@ -13663,7 +13720,9 @@
         <v>0</v>
       </c>
       <c r="AO18" s="53"/>
-      <c r="AP18" s="53"/>
+      <c r="AP18" s="53">
+        <v>2</v>
+      </c>
       <c r="AQ18" s="53"/>
       <c r="AR18" s="53"/>
       <c r="AS18" s="53"/>
@@ -13788,7 +13847,9 @@
         <v>3</v>
       </c>
       <c r="AO19" s="40"/>
-      <c r="AP19" s="40"/>
+      <c r="AP19" s="40">
+        <v>0</v>
+      </c>
       <c r="AQ19" s="40"/>
       <c r="AR19" s="40"/>
       <c r="AS19" s="40"/>
@@ -13921,7 +13982,9 @@
         <v>8</v>
       </c>
       <c r="AO20" s="6"/>
-      <c r="AP20" s="6"/>
+      <c r="AP20" s="6">
+        <v>1</v>
+      </c>
       <c r="AQ20" s="6"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="6"/>
@@ -14042,7 +14105,9 @@
       </c>
       <c r="AN21" s="51"/>
       <c r="AO21" s="51"/>
-      <c r="AP21" s="51"/>
+      <c r="AP21" s="40">
+        <v>0</v>
+      </c>
       <c r="AQ21" s="51"/>
       <c r="AR21" s="51"/>
       <c r="AS21" s="51"/>
@@ -14167,7 +14232,9 @@
       <c r="AM22" s="51"/>
       <c r="AN22" s="51"/>
       <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
+      <c r="AP22" s="40">
+        <v>0</v>
+      </c>
       <c r="AQ22" s="51"/>
       <c r="AR22" s="51"/>
       <c r="AS22" s="51"/>
@@ -14292,7 +14359,9 @@
       <c r="AM23" s="53"/>
       <c r="AN23" s="53"/>
       <c r="AO23" s="53"/>
-      <c r="AP23" s="53"/>
+      <c r="AP23" s="53">
+        <v>0</v>
+      </c>
       <c r="AQ23" s="53"/>
       <c r="AR23" s="53"/>
       <c r="AS23" s="53"/>

</xml_diff>